<commit_message>
- update plan and script header to remove jira and zephyr
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/support/empty/artifact/script/empty.xlsx
+++ b/support/empty/artifact/script/empty.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10305"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/support/empty/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B23D6D-5293-B042-887C-BDC63761949C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BB5D1C-C040-054D-9BF5-5C8F718671A3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="25080" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <definedName name="ws">'#system'!$T$2:$T$16</definedName>
     <definedName name="xml">'#system'!$U$2:$U$11</definedName>
   </definedNames>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -3322,7 +3322,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>